<commit_message>
updated editing test case in about us feature
</commit_message>
<xml_diff>
--- a/Utilities/AboutUsInput.xlsx
+++ b/Utilities/AboutUsInput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SmartCliff-Admin-Project\Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167B444F-5D8D-44AD-A8C5-6B72700DC0D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E448919C-708E-4468-88C8-48BF5AF54032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3600" yWindow="2208" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>${content_text}</t>
   </si>
@@ -49,6 +49,33 @@
   </si>
   <si>
     <t>empty_image</t>
+  </si>
+  <si>
+    <t>empty image</t>
+  </si>
+  <si>
+    <t>removing image</t>
+  </si>
+  <si>
+    <t>remove_image</t>
+  </si>
+  <si>
+    <t>same_title</t>
+  </si>
+  <si>
+    <t>test case 1</t>
+  </si>
+  <si>
+    <t>edit_new_title</t>
+  </si>
+  <si>
+    <t>sample editing test case</t>
+  </si>
+  <si>
+    <t>${new_title}</t>
+  </si>
+  <si>
+    <t>new title</t>
   </si>
 </sst>
 </file>
@@ -366,27 +393,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.21875" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -394,7 +425,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -402,14 +433,44 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
       <c r="B5" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>